<commit_message>
Vedor Pincode Mapping Template Layout changes @desc: Removed extra line after header.
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Vendor_Pincode_Mapping_Template.xlsx
+++ b/application/controllers/excel-templates/Vendor_Pincode_Mapping_Template.xlsx
@@ -424,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,35 +478,35 @@
       </c>
       <c r="K1" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J2" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Upload pincode mapping changes
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Vendor_Pincode_Mapping_Template.xlsx
+++ b/application/controllers/excel-templates/Vendor_Pincode_Mapping_Template.xlsx
@@ -14,66 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>Vendor Name</t>
-  </si>
-  <si>
-    <t>Vendor _ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Appliance</t>
-  </si>
-  <si>
-    <t>Applicance_ID</t>
-  </si>
-  <si>
-    <t>Brand</t>
-  </si>
-  <si>
-    <t>Area</t>
   </si>
   <si>
     <t>Pincode</t>
   </si>
   <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>{vendor:Vendor_Name}</t>
-  </si>
-  <si>
-    <t>{vendor:Vendor_ID}</t>
-  </si>
-  <si>
     <t>{vendor:Appliance}</t>
   </si>
   <si>
-    <t>{vendor:Appliance_ID}</t>
-  </si>
-  <si>
-    <t>{vendor:Brand}</t>
-  </si>
-  <si>
-    <t>{vendor:Area}</t>
-  </si>
-  <si>
     <t>{vendor:Pincode}</t>
-  </si>
-  <si>
-    <t>{vendor:Region}</t>
-  </si>
-  <si>
-    <t>{vendor:City}</t>
-  </si>
-  <si>
-    <t>{vendor:State}</t>
   </si>
 </sst>
 </file>
@@ -117,9 +69,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,90 +381,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="99.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>